<commit_message>
UPD: HOK testCase with UPD model
</commit_message>
<xml_diff>
--- a/TestCases/primary/HOK/params.xlsx
+++ b/TestCases/primary/HOK/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\casal2-development\TestCases\primary\HOK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F663E604-74AA-4F79-9A11-2A6FC8C4ADF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2114E0-212E-498D-9CB3-F7BB5A4C5FD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{388814BF-074A-47EB-9AA3-BAC4C704308B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="192">
   <si>
     <t>catchability[CSacous].q</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>models that claimed convergence</t>
+  </si>
+  <si>
+    <t>q[SAaut].q</t>
   </si>
 </sst>
 </file>
@@ -976,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFDAFA8-7FBD-4C00-9549-CE5729C8603D}">
   <dimension ref="A1:EX14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DR1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:EB12"/>
+    <sheetView tabSelected="1" topLeftCell="DN1" workbookViewId="0">
+      <selection activeCell="EC11" sqref="EC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,387 +1027,390 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>150</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>142</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>16</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>17</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>18</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>19</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>20</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>21</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>34</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>35</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>36</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>37</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>38</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>39</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>40</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>42</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>43</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>44</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
         <v>45</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AW2" t="s">
         <v>46</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AX2" t="s">
         <v>47</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AY2" t="s">
         <v>48</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="AZ2" t="s">
         <v>146</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BA2" t="s">
         <v>147</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>49</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>50</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>51</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BE2" t="s">
         <v>52</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
         <v>53</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BG2" t="s">
         <v>54</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BH2" t="s">
         <v>55</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BI2" t="s">
         <v>56</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BJ2" t="s">
         <v>57</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BK2" t="s">
         <v>58</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BL2" t="s">
         <v>59</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
         <v>60</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
         <v>61</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BO2" t="s">
         <v>62</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BP2" t="s">
         <v>63</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BQ2" t="s">
         <v>64</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BR2" t="s">
         <v>65</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BS2" t="s">
         <v>66</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="BT2" t="s">
         <v>67</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BU2" t="s">
         <v>68</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BV2" t="s">
         <v>69</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BW2" t="s">
         <v>70</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BX2" t="s">
         <v>71</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="BY2" t="s">
         <v>72</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="BZ2" t="s">
         <v>73</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CA2" t="s">
         <v>74</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CB2" t="s">
         <v>75</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CC2" t="s">
         <v>76</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CD2" t="s">
         <v>77</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CE2" t="s">
         <v>78</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CF2" t="s">
         <v>79</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CG2" t="s">
         <v>80</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CH2" t="s">
         <v>81</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CI2" t="s">
         <v>82</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CJ2" t="s">
         <v>83</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="CK2" t="s">
         <v>84</v>
       </c>
-      <c r="CK2" t="s">
+      <c r="CL2" t="s">
         <v>85</v>
       </c>
-      <c r="CL2" t="s">
+      <c r="CM2" t="s">
         <v>86</v>
       </c>
-      <c r="CM2" t="s">
+      <c r="CN2" t="s">
         <v>87</v>
       </c>
-      <c r="CN2" t="s">
+      <c r="CO2" t="s">
         <v>88</v>
       </c>
-      <c r="CO2" t="s">
+      <c r="CP2" t="s">
         <v>148</v>
       </c>
-      <c r="CP2" t="s">
+      <c r="CQ2" t="s">
         <v>149</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="CR2" t="s">
         <v>89</v>
       </c>
-      <c r="CR2" t="s">
+      <c r="CS2" t="s">
         <v>90</v>
       </c>
-      <c r="CS2" t="s">
+      <c r="CT2" t="s">
         <v>91</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="CU2" t="s">
         <v>92</v>
       </c>
-      <c r="CU2" t="s">
+      <c r="CV2" t="s">
         <v>93</v>
       </c>
-      <c r="CV2" t="s">
+      <c r="CW2" t="s">
         <v>94</v>
       </c>
-      <c r="CW2" t="s">
+      <c r="CX2" t="s">
         <v>95</v>
       </c>
-      <c r="CX2" t="s">
+      <c r="CY2" t="s">
         <v>151</v>
       </c>
-      <c r="CY2" t="s">
+      <c r="CZ2" t="s">
         <v>152</v>
       </c>
-      <c r="CZ2" t="s">
+      <c r="DA2" t="s">
         <v>153</v>
       </c>
-      <c r="DA2" t="s">
+      <c r="DB2" t="s">
         <v>154</v>
       </c>
-      <c r="DB2" t="s">
+      <c r="DC2" t="s">
         <v>155</v>
       </c>
-      <c r="DC2" t="s">
+      <c r="DD2" t="s">
         <v>156</v>
       </c>
-      <c r="DD2" t="s">
+      <c r="DE2" t="s">
         <v>157</v>
       </c>
-      <c r="DE2" t="s">
+      <c r="DF2" t="s">
         <v>158</v>
       </c>
-      <c r="DF2" t="s">
+      <c r="DG2" t="s">
         <v>159</v>
       </c>
-      <c r="DG2" t="s">
+      <c r="DH2" t="s">
         <v>160</v>
       </c>
-      <c r="DH2" t="s">
+      <c r="DI2" t="s">
         <v>161</v>
       </c>
-      <c r="DI2" t="s">
+      <c r="DJ2" t="s">
         <v>162</v>
       </c>
-      <c r="DJ2" t="s">
+      <c r="DK2" t="s">
         <v>163</v>
       </c>
-      <c r="DK2" t="s">
+      <c r="DL2" t="s">
         <v>164</v>
       </c>
-      <c r="DL2" t="s">
+      <c r="DM2" t="s">
         <v>165</v>
       </c>
-      <c r="DM2" t="s">
+      <c r="DN2" t="s">
         <v>166</v>
       </c>
-      <c r="DN2" t="s">
+      <c r="DO2" t="s">
         <v>96</v>
       </c>
-      <c r="DO2" t="s">
+      <c r="DP2" t="s">
         <v>97</v>
       </c>
-      <c r="DP2" t="s">
+      <c r="DQ2" t="s">
         <v>98</v>
       </c>
-      <c r="DQ2" t="s">
+      <c r="DR2" t="s">
         <v>99</v>
       </c>
-      <c r="DR2" t="s">
+      <c r="DS2" t="s">
         <v>100</v>
       </c>
-      <c r="DS2" t="s">
+      <c r="DT2" t="s">
         <v>101</v>
       </c>
-      <c r="DT2" t="s">
+      <c r="DU2" t="s">
         <v>143</v>
       </c>
-      <c r="DU2" t="s">
+      <c r="DV2" t="s">
         <v>144</v>
       </c>
-      <c r="DV2" t="s">
+      <c r="DW2" t="s">
         <v>145</v>
       </c>
-      <c r="DW2" t="s">
+      <c r="DX2" t="s">
         <v>102</v>
       </c>
-      <c r="DX2" t="s">
+      <c r="DY2" t="s">
         <v>103</v>
       </c>
-      <c r="DY2" t="s">
+      <c r="DZ2" t="s">
         <v>104</v>
       </c>
-      <c r="DZ2" t="s">
+      <c r="EA2" t="s">
         <v>105</v>
       </c>
-      <c r="EA2" t="s">
+      <c r="EB2" t="s">
         <v>106</v>
       </c>
-      <c r="EB2" t="s">
+      <c r="EC2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1422,25 +1428,25 @@
         <v>8.5307099999999997E-2</v>
       </c>
       <c r="E3">
+        <v>7.4426500000000007E-2</v>
+      </c>
+      <c r="F3">
         <v>0.14633199999999999</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.37432799999999999</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>451777</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>858436</v>
       </c>
-      <c r="I3">
-        <v>0.14000000000000001</v>
-      </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1692,117 +1698,120 @@
         <v>1</v>
       </c>
       <c r="CQ3">
+        <v>1</v>
+      </c>
+      <c r="CR3">
         <v>0.13544300000000001</v>
       </c>
-      <c r="CR3">
+      <c r="CS3">
         <v>5.1790200000000002E-2</v>
       </c>
-      <c r="CS3">
+      <c r="CT3">
         <v>0.264679</v>
       </c>
-      <c r="CT3">
+      <c r="CU3">
         <v>0.36685200000000001</v>
       </c>
-      <c r="CU3">
+      <c r="CV3">
         <v>0.32074599999999998</v>
       </c>
-      <c r="CV3">
+      <c r="CW3">
         <v>0.71906899999999996</v>
       </c>
-      <c r="CW3">
+      <c r="CX3">
         <v>0.99999899999999997</v>
       </c>
-      <c r="CX3">
+      <c r="CY3">
         <v>2.60071E-3</v>
       </c>
-      <c r="CY3">
+      <c r="CZ3">
         <v>0.13190299999999999</v>
       </c>
-      <c r="CZ3">
+      <c r="DA3">
         <v>0.419269</v>
       </c>
-      <c r="DA3">
+      <c r="DB3">
         <v>0.65148499999999998</v>
       </c>
-      <c r="DB3">
+      <c r="DC3">
         <v>0.65692499999999998</v>
       </c>
-      <c r="DC3">
+      <c r="DD3">
         <v>0.74057600000000001</v>
       </c>
-      <c r="DD3">
+      <c r="DE3">
         <v>0.82054499999999997</v>
       </c>
-      <c r="DE3">
+      <c r="DF3">
         <v>0.56485600000000002</v>
       </c>
-      <c r="DF3">
+      <c r="DG3">
         <v>0.21815999999999999</v>
       </c>
-      <c r="DG3">
+      <c r="DH3">
         <v>0.67169599999999996</v>
       </c>
-      <c r="DH3">
+      <c r="DI3">
         <v>0.778671</v>
       </c>
-      <c r="DI3">
+      <c r="DJ3">
         <v>0.80115899999999995</v>
       </c>
-      <c r="DJ3">
+      <c r="DK3">
         <v>0.86784799999999995</v>
       </c>
-      <c r="DK3">
+      <c r="DL3">
         <v>0.74476299999999995</v>
       </c>
-      <c r="DL3">
+      <c r="DM3">
         <v>0.63794899999999999</v>
       </c>
-      <c r="DM3">
+      <c r="DN3">
         <v>0.54174800000000001</v>
       </c>
-      <c r="DN3">
-        <v>34</v>
-      </c>
       <c r="DO3">
+        <v>14</v>
+      </c>
+      <c r="DP3">
         <v>10.7575</v>
       </c>
-      <c r="DP3">
+      <c r="DQ3">
         <v>44</v>
       </c>
-      <c r="DQ3">
-        <v>34</v>
-      </c>
       <c r="DR3">
+        <v>14</v>
+      </c>
+      <c r="DS3">
         <v>12.6136</v>
       </c>
-      <c r="DS3">
+      <c r="DT3">
         <v>27.035799999999998</v>
       </c>
-      <c r="DT3">
-        <v>34</v>
-      </c>
       <c r="DU3">
+        <v>14</v>
+      </c>
+      <c r="DV3">
         <v>12.6136</v>
       </c>
-      <c r="DV3">
+      <c r="DW3">
         <v>27.035799999999998</v>
       </c>
-      <c r="DW3">
-        <v>34</v>
-      </c>
       <c r="DX3">
+        <v>14</v>
+      </c>
+      <c r="DY3">
         <v>17.063099999999999</v>
       </c>
-      <c r="DY3">
+      <c r="DZ3">
         <v>38.280299999999997</v>
       </c>
-      <c r="DZ3">
-        <v>34</v>
-      </c>
       <c r="EA3">
+        <v>14</v>
+      </c>
+      <c r="EB3">
         <v>44</v>
       </c>
-      <c r="EB3">
+      <c r="EC3">
         <v>44</v>
       </c>
     </row>
@@ -1825,483 +1834,489 @@
         <v>114</v>
       </c>
       <c r="E6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" t="s">
         <v>115</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>116</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>117</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>118</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>119</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>120</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>121</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>42</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>122</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>42</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>123</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>8</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>124</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>8</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>125</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>8</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>126</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>3</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>127</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>3</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>128</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>3</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>129</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>3</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>130</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.42803000000000002</v>
+        <v>1.22472</v>
       </c>
       <c r="B7">
-        <v>0.26921800000000001</v>
+        <v>0.93811199999999995</v>
       </c>
       <c r="C7">
-        <v>7.82389E-2</v>
+        <v>8.0427600000000002E-2</v>
       </c>
       <c r="D7">
-        <v>5.1318200000000001E-2</v>
+        <v>0.109987</v>
       </c>
       <c r="E7">
-        <v>0.140235</v>
+        <v>8.7812799999999996E-2</v>
       </c>
       <c r="F7">
-        <v>0.42616300000000001</v>
+        <v>0.14633199999999999</v>
       </c>
       <c r="G7">
-        <v>14.411899999999999</v>
+        <v>0.37432799999999999</v>
       </c>
       <c r="H7">
-        <v>0.31486799999999998</v>
+        <v>13.9</v>
       </c>
       <c r="I7">
-        <v>0.28209000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="J7">
-        <v>-0.204433</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="K7">
-        <v>0.45374900000000001</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>0.73531100000000005</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>0.78877600000000003</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>1.3609500000000001</v>
+        <v>1</v>
       </c>
       <c r="O7">
-        <v>0.99126300000000001</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>0.32924500000000001</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>0.44685399999999997</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>0.26535599999999998</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>0.43360500000000002</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>0.48915599999999998</v>
+        <v>1</v>
       </c>
       <c r="U7">
-        <v>0.39713599999999999</v>
+        <v>1</v>
       </c>
       <c r="V7">
-        <v>0.218279</v>
+        <v>1</v>
       </c>
       <c r="W7">
-        <v>1.03389</v>
+        <v>1</v>
       </c>
       <c r="X7">
-        <v>0.97579000000000005</v>
+        <v>1</v>
       </c>
       <c r="Y7">
-        <v>0.43847999999999998</v>
+        <v>1</v>
       </c>
       <c r="Z7">
-        <v>0.14163000000000001</v>
+        <v>1</v>
       </c>
       <c r="AA7">
-        <v>0.37155100000000002</v>
+        <v>1</v>
       </c>
       <c r="AB7">
-        <v>0.40284500000000001</v>
+        <v>1</v>
       </c>
       <c r="AC7">
-        <v>0.386654</v>
+        <v>1</v>
       </c>
       <c r="AD7">
-        <v>0.54398400000000002</v>
+        <v>1</v>
       </c>
       <c r="AE7">
-        <v>0.27254099999999998</v>
+        <v>1</v>
       </c>
       <c r="AF7">
-        <v>0.27902399999999999</v>
+        <v>1</v>
       </c>
       <c r="AG7">
-        <v>0.44855099999999998</v>
+        <v>1</v>
       </c>
       <c r="AH7">
-        <v>0.24976100000000001</v>
+        <v>1</v>
       </c>
       <c r="AI7">
-        <v>0.06</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
-        <v>0.45893</v>
+        <v>1</v>
       </c>
       <c r="AK7">
-        <v>0.161166</v>
+        <v>1</v>
       </c>
       <c r="AL7">
-        <v>0.26452100000000001</v>
+        <v>1</v>
       </c>
       <c r="AM7">
-        <v>0.49690299999999998</v>
+        <v>1</v>
       </c>
       <c r="AN7">
-        <v>0.51354599999999995</v>
+        <v>1</v>
       </c>
       <c r="AO7">
-        <v>0.50587000000000004</v>
+        <v>1</v>
       </c>
       <c r="AP7">
-        <v>0.595028</v>
+        <v>1</v>
       </c>
       <c r="AQ7">
-        <v>0.52052100000000001</v>
+        <v>1</v>
       </c>
       <c r="AR7">
-        <v>0.37137999999999999</v>
+        <v>1</v>
       </c>
       <c r="AS7">
-        <v>0.51846300000000001</v>
+        <v>1</v>
       </c>
       <c r="AT7">
-        <v>0.16014100000000001</v>
+        <v>1</v>
       </c>
       <c r="AU7">
-        <v>0.65075700000000003</v>
+        <v>1</v>
       </c>
       <c r="AV7">
-        <v>0.15484100000000001</v>
+        <v>1</v>
       </c>
       <c r="AW7">
-        <v>0.18554599999999999</v>
+        <v>1</v>
       </c>
       <c r="AX7">
-        <v>0.71806300000000001</v>
+        <v>1</v>
       </c>
       <c r="AY7">
-        <v>0.687504</v>
+        <v>1</v>
       </c>
       <c r="AZ7">
-        <v>1.19232</v>
+        <v>1</v>
       </c>
       <c r="BA7">
-        <v>0.470084</v>
+        <v>1</v>
       </c>
       <c r="BB7">
-        <v>0.87542299999999995</v>
+        <v>1</v>
       </c>
       <c r="BC7">
-        <v>0.69200700000000004</v>
+        <v>1</v>
       </c>
       <c r="BD7">
-        <v>0.67660200000000004</v>
+        <v>1</v>
       </c>
       <c r="BE7">
-        <v>0.48854199999999998</v>
+        <v>1</v>
       </c>
       <c r="BF7">
-        <v>0.53743200000000002</v>
+        <v>1</v>
       </c>
       <c r="BG7">
-        <v>0.61270500000000006</v>
+        <v>1</v>
       </c>
       <c r="BH7">
-        <v>0.51178599999999996</v>
+        <v>1</v>
       </c>
       <c r="BI7">
-        <v>0.91530299999999998</v>
+        <v>1</v>
       </c>
       <c r="BJ7">
-        <v>0.86049500000000001</v>
+        <v>1</v>
       </c>
       <c r="BK7">
-        <v>0.35201700000000002</v>
+        <v>1</v>
       </c>
       <c r="BL7">
-        <v>0.14932699999999999</v>
+        <v>1</v>
       </c>
       <c r="BM7">
-        <v>1.25695</v>
+        <v>1</v>
       </c>
       <c r="BN7">
-        <v>0.68313900000000005</v>
+        <v>1</v>
       </c>
       <c r="BO7">
-        <v>0.141293</v>
+        <v>1</v>
       </c>
       <c r="BP7">
-        <v>8.2569799999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="BQ7">
-        <v>0.87184300000000003</v>
+        <v>1</v>
       </c>
       <c r="BR7">
-        <v>1.07863</v>
+        <v>1</v>
       </c>
       <c r="BS7">
-        <v>0.355902</v>
+        <v>1</v>
       </c>
       <c r="BT7">
-        <v>1.01223</v>
+        <v>1</v>
       </c>
       <c r="BU7">
-        <v>0.15787200000000001</v>
+        <v>1</v>
       </c>
       <c r="BV7">
-        <v>0.22095699999999999</v>
+        <v>1</v>
       </c>
       <c r="BW7">
-        <v>0.22945299999999999</v>
+        <v>1</v>
       </c>
       <c r="BX7">
-        <v>0.20191200000000001</v>
+        <v>1</v>
       </c>
       <c r="BY7">
-        <v>0.06</v>
+        <v>1</v>
       </c>
       <c r="BZ7">
-        <v>0.36727900000000002</v>
+        <v>1</v>
       </c>
       <c r="CA7">
-        <v>9.44657E-2</v>
+        <v>1</v>
       </c>
       <c r="CB7">
-        <v>0.78962900000000003</v>
+        <v>1</v>
       </c>
       <c r="CC7">
-        <v>0.46132099999999998</v>
+        <v>1</v>
       </c>
       <c r="CD7">
-        <v>0.51471100000000003</v>
+        <v>1</v>
       </c>
       <c r="CE7">
-        <v>0.50687300000000002</v>
+        <v>1</v>
       </c>
       <c r="CF7">
-        <v>0.752637</v>
+        <v>1</v>
       </c>
       <c r="CG7">
-        <v>0.63731199999999999</v>
+        <v>1</v>
       </c>
       <c r="CH7">
-        <v>0.61607699999999999</v>
+        <v>1</v>
       </c>
       <c r="CI7">
-        <v>0.58324399999999998</v>
+        <v>1</v>
       </c>
       <c r="CJ7">
-        <v>0.140766</v>
+        <v>1</v>
       </c>
       <c r="CK7">
-        <v>0.98051699999999997</v>
+        <v>1</v>
       </c>
       <c r="CL7">
-        <v>0.15967799999999999</v>
+        <v>1</v>
       </c>
       <c r="CM7">
-        <v>0.23666300000000001</v>
+        <v>1</v>
       </c>
       <c r="CN7">
-        <v>2.2108699999999999</v>
+        <v>1</v>
       </c>
       <c r="CO7">
-        <v>2.1520899999999998</v>
+        <v>1</v>
       </c>
       <c r="CP7">
-        <v>1.19258</v>
+        <v>1</v>
       </c>
       <c r="CQ7">
-        <v>0.319604</v>
+        <v>1</v>
       </c>
       <c r="CR7">
-        <v>0.34394799999999998</v>
+        <v>0.1</v>
       </c>
       <c r="CS7">
-        <v>0.55652500000000005</v>
+        <v>0.1</v>
       </c>
       <c r="CT7" s="2">
-        <v>1.27257E-8</v>
+        <v>0.43</v>
       </c>
       <c r="CU7">
-        <v>0.63922199999999996</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="CV7">
-        <v>0.78522099999999995</v>
+        <v>0.88</v>
       </c>
       <c r="CW7" s="2">
-        <v>8.3693499999999994E-8</v>
+        <v>0.9</v>
       </c>
       <c r="CX7">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="CY7">
-        <v>5.5405200000000002E-3</v>
+        <v>1</v>
       </c>
       <c r="CZ7">
-        <v>0.15859500000000001</v>
+        <v>0.1</v>
       </c>
       <c r="DA7">
-        <v>0.32335399999999997</v>
+        <v>0.2</v>
       </c>
       <c r="DB7">
-        <v>0.43395499999999998</v>
+        <v>0.3</v>
       </c>
       <c r="DC7">
-        <v>0.38996999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="DD7">
-        <v>0.47155399999999997</v>
+        <v>0.5</v>
       </c>
       <c r="DE7">
-        <v>0.60818899999999998</v>
+        <v>0.6</v>
       </c>
       <c r="DF7">
-        <v>0.60419199999999995</v>
+        <v>0.6</v>
       </c>
       <c r="DG7">
-        <v>0.11063099999999999</v>
+        <v>0.6</v>
       </c>
       <c r="DH7">
-        <v>0.28572199999999998</v>
+        <v>0.1</v>
       </c>
       <c r="DI7">
-        <v>0.26705499999999999</v>
+        <v>0.2</v>
       </c>
       <c r="DJ7">
-        <v>0.46222200000000002</v>
+        <v>0.3</v>
       </c>
       <c r="DK7">
-        <v>0.48046699999999998</v>
+        <v>0.4</v>
       </c>
       <c r="DL7">
-        <v>0.52906600000000004</v>
+        <v>0.5</v>
       </c>
       <c r="DM7">
-        <v>0.67556799999999995</v>
+        <v>0.6</v>
       </c>
       <c r="DN7">
-        <v>0.58922200000000002</v>
+        <v>0.6</v>
       </c>
       <c r="DO7">
-        <v>3.6044800000000001</v>
+        <v>0.6</v>
       </c>
       <c r="DP7">
-        <v>1.2138599999999999</v>
+        <v>3.82578</v>
       </c>
       <c r="DQ7">
-        <v>12.3926</v>
+        <v>1.6303799999999999</v>
       </c>
       <c r="DR7">
-        <v>10.2812</v>
+        <v>17</v>
       </c>
       <c r="DS7">
-        <v>7.9295900000000001</v>
+        <v>5.34802</v>
       </c>
       <c r="DT7">
-        <v>4.7031000000000001</v>
+        <v>2.1239599999999998</v>
       </c>
       <c r="DU7">
-        <v>10.650600000000001</v>
+        <v>7.7964700000000002</v>
       </c>
       <c r="DV7">
-        <v>13.4466</v>
+        <v>10.6006</v>
       </c>
       <c r="DW7">
-        <v>3.8997600000000001</v>
+        <v>7.58432</v>
       </c>
       <c r="DX7">
-        <v>1</v>
+        <v>3.6039500000000002</v>
       </c>
       <c r="DY7">
-        <v>1</v>
+        <v>1.0007999999999999</v>
       </c>
       <c r="DZ7">
-        <v>8.9715000000000007</v>
+        <v>1</v>
       </c>
       <c r="EA7">
-        <v>14.2028</v>
+        <v>8.7178100000000001</v>
       </c>
       <c r="EB7">
-        <v>9.2013800000000003</v>
+        <v>10</v>
       </c>
       <c r="EC7">
-        <v>1.29365</v>
+        <v>5.5027999999999997</v>
+      </c>
+      <c r="ED7">
+        <v>3.2463500000000001</v>
       </c>
     </row>
     <row r="9" spans="1:154" x14ac:dyDescent="0.25">
@@ -2327,1052 +2342,1059 @@
         <v>catchability[SAsum].q</v>
       </c>
       <c r="E11" t="str">
-        <f>E2</f>
+        <f t="shared" ref="E11:AJ11" si="1">E2</f>
+        <v>catchability[SAaut].q</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
         <v>observation[CRsumbio].process_error</v>
       </c>
-      <c r="F11" t="str">
-        <f>F2</f>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
         <v>observation[SAsumbio].process_error</v>
       </c>
-      <c r="G11" t="str">
-        <f>G2</f>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].b0</v>
       </c>
-      <c r="H11" t="str">
-        <f>H2</f>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_W].b0</v>
       </c>
-      <c r="I11" t="str">
-        <f>I2</f>
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
         <v>process[Instant_mortality].m{west.sa}</v>
       </c>
-      <c r="J11" t="str">
-        <f>J2</f>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
         <v>time_varying[shifted_mu].a</v>
       </c>
-      <c r="K11" t="str">
-        <f>K2</f>
+      <c r="L11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1975}</v>
       </c>
-      <c r="L11" t="str">
-        <f>L2</f>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1976}</v>
       </c>
-      <c r="M11" t="str">
-        <f>M2</f>
+      <c r="N11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1977}</v>
       </c>
-      <c r="N11" t="str">
-        <f>N2</f>
+      <c r="O11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1978}</v>
       </c>
-      <c r="O11" t="str">
-        <f>O2</f>
+      <c r="P11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1979}</v>
       </c>
-      <c r="P11" t="str">
-        <f>P2</f>
+      <c r="Q11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1980}</v>
       </c>
-      <c r="Q11" t="str">
-        <f>Q2</f>
+      <c r="R11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1981}</v>
       </c>
-      <c r="R11" t="str">
-        <f>R2</f>
+      <c r="S11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1982}</v>
       </c>
-      <c r="S11" t="str">
-        <f>S2</f>
+      <c r="T11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1983}</v>
       </c>
-      <c r="T11" t="str">
-        <f>T2</f>
+      <c r="U11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1984}</v>
       </c>
-      <c r="U11" t="str">
-        <f>U2</f>
+      <c r="V11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1985}</v>
       </c>
-      <c r="V11" t="str">
-        <f>V2</f>
+      <c r="W11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1986}</v>
       </c>
-      <c r="W11" t="str">
-        <f>W2</f>
+      <c r="X11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1987}</v>
       </c>
-      <c r="X11" t="str">
-        <f>X2</f>
+      <c r="Y11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1988}</v>
       </c>
-      <c r="Y11" t="str">
-        <f>Y2</f>
+      <c r="Z11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1989}</v>
       </c>
-      <c r="Z11" t="str">
-        <f>Z2</f>
+      <c r="AA11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1990}</v>
       </c>
-      <c r="AA11" t="str">
-        <f>AA2</f>
+      <c r="AB11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1991}</v>
       </c>
-      <c r="AB11" t="str">
-        <f>AB2</f>
+      <c r="AC11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1992}</v>
       </c>
-      <c r="AC11" t="str">
-        <f>AC2</f>
+      <c r="AD11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1993}</v>
       </c>
-      <c r="AD11" t="str">
-        <f>AD2</f>
+      <c r="AE11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1994}</v>
       </c>
-      <c r="AE11" t="str">
-        <f>AE2</f>
+      <c r="AF11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1995}</v>
       </c>
-      <c r="AF11" t="str">
-        <f>AF2</f>
+      <c r="AG11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1996}</v>
       </c>
-      <c r="AG11" t="str">
-        <f>AG2</f>
+      <c r="AH11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1997}</v>
       </c>
-      <c r="AH11" t="str">
-        <f>AH2</f>
+      <c r="AI11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1998}</v>
       </c>
-      <c r="AI11" t="str">
-        <f>AI2</f>
+      <c r="AJ11" t="str">
+        <f t="shared" si="1"/>
         <v>process[recruit_E].ycs_values{1999}</v>
       </c>
-      <c r="AJ11" t="str">
-        <f>AJ2</f>
+      <c r="AK11" t="str">
+        <f t="shared" ref="AK11:BL11" si="2">AK2</f>
         <v>process[recruit_E].ycs_values{2000}</v>
       </c>
-      <c r="AK11" t="str">
-        <f>AK2</f>
+      <c r="AL11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2001}</v>
       </c>
-      <c r="AL11" t="str">
-        <f>AL2</f>
+      <c r="AM11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2002}</v>
       </c>
-      <c r="AM11" t="str">
-        <f>AM2</f>
+      <c r="AN11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2003}</v>
       </c>
-      <c r="AN11" t="str">
-        <f>AN2</f>
+      <c r="AO11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2004}</v>
       </c>
-      <c r="AO11" t="str">
-        <f>AO2</f>
+      <c r="AP11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2005}</v>
       </c>
-      <c r="AP11" t="str">
-        <f>AP2</f>
+      <c r="AQ11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2006}</v>
       </c>
-      <c r="AQ11" t="str">
-        <f>AQ2</f>
+      <c r="AR11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2007}</v>
       </c>
-      <c r="AR11" t="str">
-        <f>AR2</f>
+      <c r="AS11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2008}</v>
       </c>
-      <c r="AS11" t="str">
-        <f>AS2</f>
+      <c r="AT11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2009}</v>
       </c>
-      <c r="AT11" t="str">
-        <f>AT2</f>
+      <c r="AU11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2010}</v>
       </c>
-      <c r="AU11" t="str">
-        <f>AU2</f>
+      <c r="AV11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2011}</v>
       </c>
-      <c r="AV11" t="str">
-        <f>AV2</f>
+      <c r="AW11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2012}</v>
       </c>
-      <c r="AW11" t="str">
-        <f>AW2</f>
+      <c r="AX11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2013}</v>
       </c>
-      <c r="AX11" t="str">
-        <f>AX2</f>
+      <c r="AY11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2014}</v>
       </c>
-      <c r="AY11" t="str">
-        <f>AY2</f>
+      <c r="AZ11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2015}</v>
       </c>
-      <c r="AZ11" t="str">
-        <f>AZ2</f>
+      <c r="BA11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_E].ycs_values{2016}</v>
       </c>
-      <c r="BA11" t="str">
-        <f>BA2</f>
+      <c r="BB11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1975}</v>
       </c>
-      <c r="BB11" t="str">
-        <f>BB2</f>
+      <c r="BC11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1976}</v>
       </c>
-      <c r="BC11" t="str">
-        <f>BC2</f>
+      <c r="BD11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1977}</v>
       </c>
-      <c r="BD11" t="str">
-        <f>BD2</f>
+      <c r="BE11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1978}</v>
       </c>
-      <c r="BE11" t="str">
-        <f>BE2</f>
+      <c r="BF11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1979}</v>
       </c>
-      <c r="BF11" t="str">
-        <f>BF2</f>
+      <c r="BG11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1980}</v>
       </c>
-      <c r="BG11" t="str">
-        <f>BG2</f>
+      <c r="BH11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1981}</v>
       </c>
-      <c r="BH11" t="str">
-        <f>BH2</f>
+      <c r="BI11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1982}</v>
       </c>
-      <c r="BI11" t="str">
-        <f>BI2</f>
+      <c r="BJ11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1983}</v>
       </c>
-      <c r="BJ11" t="str">
-        <f>BJ2</f>
+      <c r="BK11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1984}</v>
       </c>
-      <c r="BK11" t="str">
-        <f>BK2</f>
+      <c r="BL11" t="str">
+        <f t="shared" si="2"/>
         <v>process[recruit_W].ycs_values{1985}</v>
       </c>
-      <c r="BL11" t="str">
-        <f>BL2</f>
+      <c r="BM11" t="str">
+        <f t="shared" ref="BM11:DX11" si="3">BM2</f>
         <v>process[recruit_W].ycs_values{1986}</v>
       </c>
-      <c r="BM11" t="str">
-        <f t="shared" ref="BM11:DX11" si="1">BM2</f>
+      <c r="BN11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1987}</v>
       </c>
-      <c r="BN11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BO11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1988}</v>
       </c>
-      <c r="BO11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BP11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1989}</v>
       </c>
-      <c r="BP11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BQ11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1990}</v>
       </c>
-      <c r="BQ11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BR11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1991}</v>
       </c>
-      <c r="BR11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BS11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1992}</v>
       </c>
-      <c r="BS11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BT11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1993}</v>
       </c>
-      <c r="BT11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BU11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1994}</v>
       </c>
-      <c r="BU11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BV11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1995}</v>
       </c>
-      <c r="BV11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BW11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1996}</v>
       </c>
-      <c r="BW11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BX11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1997}</v>
       </c>
-      <c r="BX11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BY11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1998}</v>
       </c>
-      <c r="BY11" t="str">
-        <f t="shared" si="1"/>
+      <c r="BZ11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{1999}</v>
       </c>
-      <c r="BZ11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CA11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2000}</v>
       </c>
-      <c r="CA11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CB11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2001}</v>
       </c>
-      <c r="CB11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CC11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2002}</v>
       </c>
-      <c r="CC11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CD11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2003}</v>
       </c>
-      <c r="CD11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CE11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2004}</v>
       </c>
-      <c r="CE11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CF11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2005}</v>
       </c>
-      <c r="CF11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CG11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2006}</v>
       </c>
-      <c r="CG11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CH11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2007}</v>
       </c>
-      <c r="CH11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CI11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2008}</v>
       </c>
-      <c r="CI11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CJ11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2009}</v>
       </c>
-      <c r="CJ11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CK11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2010}</v>
       </c>
-      <c r="CK11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CL11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2011}</v>
       </c>
-      <c r="CL11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CM11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2012}</v>
       </c>
-      <c r="CM11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CN11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2013}</v>
       </c>
-      <c r="CN11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CO11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2014}</v>
       </c>
-      <c r="CO11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CP11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2015}</v>
       </c>
-      <c r="CP11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CQ11" t="str">
+        <f t="shared" si="3"/>
         <v>process[recruit_W].ycs_values{2016}</v>
       </c>
-      <c r="CQ11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CR11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Whome].v{1}</v>
       </c>
-      <c r="CR11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CS11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Whome].v{2}</v>
       </c>
-      <c r="CS11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CT11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Whome].v{3}</v>
       </c>
-      <c r="CT11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CU11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Whome].v{4}</v>
       </c>
-      <c r="CU11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CV11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Whome].v{5}</v>
       </c>
-      <c r="CV11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CW11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Whome].v{6}</v>
       </c>
-      <c r="CW11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CX11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Whome].v{7}</v>
       </c>
-      <c r="CX11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CY11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Espmg].v{1}</v>
       </c>
-      <c r="CY11" t="str">
-        <f t="shared" si="1"/>
+      <c r="CZ11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Espmg].v{2}</v>
       </c>
-      <c r="CZ11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DA11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Espmg].v{3}</v>
       </c>
-      <c r="DA11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DB11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Espmg].v{4}</v>
       </c>
-      <c r="DB11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DC11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Espmg].v{5}</v>
       </c>
-      <c r="DC11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DD11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Espmg].v{6}</v>
       </c>
-      <c r="DD11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DE11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Espmg].v{7}</v>
       </c>
-      <c r="DE11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DF11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Espmg].v{8}</v>
       </c>
-      <c r="DF11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DG11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Wspmg].v{1}</v>
       </c>
-      <c r="DG11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DH11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Wspmg].v{2}</v>
       </c>
-      <c r="DH11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DI11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Wspmg].v{3}</v>
       </c>
-      <c r="DI11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DJ11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Wspmg].v{4}</v>
       </c>
-      <c r="DJ11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DK11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Wspmg].v{5}</v>
       </c>
-      <c r="DK11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DL11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Wspmg].v{6}</v>
       </c>
-      <c r="DL11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DM11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Wspmg].v{7}</v>
       </c>
-      <c r="DM11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DN11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[sel_Wspmg].v{8}</v>
       </c>
-      <c r="DN11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DO11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[Enspsl].mu</v>
       </c>
-      <c r="DO11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DP11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[Enspsl].sigma_l</v>
       </c>
-      <c r="DP11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DQ11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[Enspsl].sigma_r</v>
       </c>
-      <c r="DQ11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DR11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[Wnspsl].mu</v>
       </c>
-      <c r="DR11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DS11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[Wnspsl].sigma_l</v>
       </c>
-      <c r="DS11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DT11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[Wnspsl].sigma_r</v>
       </c>
-      <c r="DT11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DU11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[Espsl].mu</v>
       </c>
-      <c r="DU11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DV11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[Espsl].sigma_l</v>
       </c>
-      <c r="DV11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DW11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[Espsl].sigma_r</v>
       </c>
-      <c r="DW11" t="str">
-        <f t="shared" si="1"/>
+      <c r="DX11" t="str">
+        <f t="shared" si="3"/>
         <v>selectivity[CRsl].mu</v>
-      </c>
-      <c r="DX11" t="str">
-        <f t="shared" si="1"/>
-        <v>selectivity[CRsl].sigma_l</v>
       </c>
       <c r="DY11" t="str">
         <f>DY2</f>
-        <v>selectivity[CRsl].sigma_r</v>
+        <v>selectivity[CRsl].sigma_l</v>
       </c>
       <c r="DZ11" t="str">
         <f>DZ2</f>
-        <v>selectivity[SAsl].mu</v>
+        <v>selectivity[CRsl].sigma_r</v>
       </c>
       <c r="EA11" t="str">
         <f>EA2</f>
-        <v>selectivity[SAsl].sigma_l</v>
+        <v>selectivity[SAsl].mu</v>
       </c>
       <c r="EB11" t="str">
         <f>EB2</f>
+        <v>selectivity[SAsl].sigma_l</v>
+      </c>
+      <c r="EC11" t="str">
+        <f>EC2</f>
         <v>selectivity[SAsl].sigma_r</v>
       </c>
       <c r="EX11">
-        <f t="shared" ref="EX11" si="2">EX2</f>
+        <f t="shared" ref="EX11" si="4">EX2</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f>A7</f>
-        <v>0.42803000000000002</v>
+        <v>1.22472</v>
       </c>
       <c r="B12" s="4">
-        <f t="shared" ref="B12:D12" si="3">B7</f>
-        <v>0.26921800000000001</v>
+        <f t="shared" ref="B12:D12" si="5">B7</f>
+        <v>0.93811199999999995</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" si="3"/>
-        <v>7.82389E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.0427600000000002E-2</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="3"/>
-        <v>5.1318200000000001E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.109987</v>
       </c>
       <c r="E12" s="4">
         <f>E7</f>
-        <v>0.140235</v>
+        <v>8.7812799999999996E-2</v>
       </c>
       <c r="F12" s="4">
         <f>F7</f>
-        <v>0.42616300000000001</v>
-      </c>
-      <c r="G12" s="3">
-        <f>EXP(G7) * H7</f>
-        <v>571659.16329672444</v>
+        <v>0.14633199999999999</v>
+      </c>
+      <c r="G12" s="4">
+        <f>G7</f>
+        <v>0.37432799999999999</v>
       </c>
       <c r="H12" s="3">
-        <f>EXP(G7) * (1 - H7)</f>
-        <v>1243892.6339539473</v>
-      </c>
-      <c r="I12" s="4">
-        <f>I7</f>
-        <v>0.28209000000000001</v>
+        <f>EXP(H7) *I7</f>
+        <v>272040.33885066013</v>
+      </c>
+      <c r="I12" s="3">
+        <f>EXP(H7) *(1-I7)</f>
+        <v>816121.0165519804</v>
       </c>
       <c r="J12" s="4">
         <f>J7</f>
-        <v>-0.204433</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="K12" s="4">
         <f>K7</f>
-        <v>0.45374900000000001</v>
+        <v>0</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" ref="L12:BW12" si="4">L7</f>
-        <v>0.73531100000000005</v>
+        <f t="shared" ref="L12:BW12" si="6">L7</f>
+        <v>1</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.78877600000000003</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3609500000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99126300000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.32924500000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.44685399999999997</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="R12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.26535599999999998</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="S12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.43360500000000002</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="T12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.48915599999999998</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="U12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.39713599999999999</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="V12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.218279</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="W12" s="4">
-        <f t="shared" si="4"/>
-        <v>1.03389</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="X12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.97579000000000005</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="Y12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.43847999999999998</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="Z12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.14163000000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AA12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.37155100000000002</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AB12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.40284500000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AC12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.386654</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AD12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.54398400000000002</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AE12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.27254099999999998</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AF12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.27902399999999999</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AG12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.44855099999999998</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AH12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.24976100000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AI12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.06</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AJ12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.45893</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AK12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.161166</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AL12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.26452100000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AM12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.49690299999999998</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AN12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.51354599999999995</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AO12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.50587000000000004</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AP12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.595028</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AQ12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.52052100000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AR12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.37137999999999999</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AS12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.51846300000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AT12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.16014100000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AU12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.65075700000000003</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AV12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.15484100000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AW12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.18554599999999999</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AX12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.71806300000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AY12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.687504</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AZ12" s="4">
-        <f t="shared" si="4"/>
-        <v>1.19232</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BA12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.470084</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BB12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.87542299999999995</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BC12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.69200700000000004</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BD12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.67660200000000004</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BE12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.48854199999999998</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BF12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.53743200000000002</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BG12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.61270500000000006</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BH12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.51178599999999996</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BI12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.91530299999999998</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BJ12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.86049500000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BK12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.35201700000000002</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BL12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.14932699999999999</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BM12" s="4">
-        <f t="shared" si="4"/>
-        <v>1.25695</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BN12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.68313900000000005</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BO12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.141293</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BP12" s="4">
-        <f t="shared" si="4"/>
-        <v>8.2569799999999999E-2</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BQ12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.87184300000000003</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BR12" s="4">
-        <f t="shared" si="4"/>
-        <v>1.07863</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BS12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.355902</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BT12" s="4">
-        <f t="shared" si="4"/>
-        <v>1.01223</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BU12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.15787200000000001</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BV12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.22095699999999999</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BW12" s="4">
-        <f t="shared" si="4"/>
-        <v>0.22945299999999999</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="BX12" s="4">
-        <f t="shared" ref="BX12:CV12" si="5">BX7</f>
-        <v>0.20191200000000001</v>
+        <f t="shared" ref="BX12:CV12" si="7">BX7</f>
+        <v>1</v>
       </c>
       <c r="BY12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.06</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="BZ12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.36727900000000002</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CA12" s="4">
-        <f t="shared" si="5"/>
-        <v>9.44657E-2</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CB12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.78962900000000003</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CC12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.46132099999999998</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CD12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.51471100000000003</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CE12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.50687300000000002</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CF12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.752637</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CG12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.63731199999999999</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CH12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.61607699999999999</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CI12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.58324399999999998</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CJ12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.140766</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CK12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.98051699999999997</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CL12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.15967799999999999</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CM12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.23666300000000001</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CN12" s="4">
-        <f t="shared" si="5"/>
-        <v>2.2108699999999999</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CO12" s="4">
-        <f t="shared" si="5"/>
-        <v>2.1520899999999998</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CP12" s="4">
-        <f t="shared" si="5"/>
-        <v>1.19258</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CQ12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.319604</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="CR12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.34394799999999998</v>
+        <f t="shared" si="7"/>
+        <v>0.1</v>
       </c>
       <c r="CS12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.55652500000000005</v>
+        <f t="shared" si="7"/>
+        <v>0.1</v>
       </c>
       <c r="CT12" s="4">
-        <f t="shared" si="5"/>
-        <v>1.27257E-8</v>
+        <f t="shared" si="7"/>
+        <v>0.43</v>
       </c>
       <c r="CU12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.63922199999999996</v>
+        <f t="shared" si="7"/>
+        <v>0.56000000000000005</v>
       </c>
       <c r="CV12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.78522099999999995</v>
+        <f t="shared" si="7"/>
+        <v>0.88</v>
       </c>
       <c r="CW12" s="4">
         <f>CW7</f>
-        <v>8.3693499999999994E-8</v>
+        <v>0.9</v>
       </c>
       <c r="CX12" s="4">
-        <f>CY7</f>
-        <v>5.5405200000000002E-3</v>
+        <f>CX7</f>
+        <v>0.95</v>
       </c>
       <c r="CY12" s="4">
-        <f t="shared" ref="CY12:EB12" si="6">CZ7</f>
-        <v>0.15859500000000001</v>
+        <f>CZ7</f>
+        <v>0.1</v>
       </c>
       <c r="CZ12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.32335399999999997</v>
+        <f t="shared" ref="CZ12:EC12" si="8">DA7</f>
+        <v>0.2</v>
       </c>
       <c r="DA12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.43395499999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.3</v>
       </c>
       <c r="DB12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.38996999999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.4</v>
       </c>
       <c r="DC12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.47155399999999997</v>
+        <f t="shared" si="8"/>
+        <v>0.5</v>
       </c>
       <c r="DD12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.60818899999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.6</v>
       </c>
       <c r="DE12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.60419199999999995</v>
+        <f t="shared" si="8"/>
+        <v>0.6</v>
       </c>
       <c r="DF12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.11063099999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.6</v>
       </c>
       <c r="DG12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.28572199999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.1</v>
       </c>
       <c r="DH12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.26705499999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.2</v>
       </c>
       <c r="DI12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.46222200000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.3</v>
       </c>
       <c r="DJ12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.48046699999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.4</v>
       </c>
       <c r="DK12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.52906600000000004</v>
+        <f t="shared" si="8"/>
+        <v>0.5</v>
       </c>
       <c r="DL12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.67556799999999995</v>
+        <f t="shared" si="8"/>
+        <v>0.6</v>
       </c>
       <c r="DM12" s="4">
-        <f t="shared" si="6"/>
-        <v>0.58922200000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.6</v>
       </c>
       <c r="DN12" s="4">
-        <f t="shared" si="6"/>
-        <v>3.6044800000000001</v>
+        <f t="shared" si="8"/>
+        <v>0.6</v>
       </c>
       <c r="DO12" s="4">
-        <f t="shared" si="6"/>
-        <v>1.2138599999999999</v>
+        <f t="shared" si="8"/>
+        <v>3.82578</v>
       </c>
       <c r="DP12" s="4">
-        <f t="shared" si="6"/>
-        <v>12.3926</v>
+        <f t="shared" si="8"/>
+        <v>1.6303799999999999</v>
       </c>
       <c r="DQ12" s="4">
-        <f t="shared" si="6"/>
-        <v>10.2812</v>
+        <f t="shared" si="8"/>
+        <v>17</v>
       </c>
       <c r="DR12" s="4">
-        <f t="shared" si="6"/>
-        <v>7.9295900000000001</v>
+        <f t="shared" si="8"/>
+        <v>5.34802</v>
       </c>
       <c r="DS12" s="4">
-        <f t="shared" si="6"/>
-        <v>4.7031000000000001</v>
+        <f t="shared" si="8"/>
+        <v>2.1239599999999998</v>
       </c>
       <c r="DT12" s="4">
-        <f t="shared" si="6"/>
-        <v>10.650600000000001</v>
+        <f t="shared" si="8"/>
+        <v>7.7964700000000002</v>
       </c>
       <c r="DU12" s="4">
-        <f t="shared" si="6"/>
-        <v>13.4466</v>
+        <f t="shared" si="8"/>
+        <v>10.6006</v>
       </c>
       <c r="DV12" s="4">
-        <f t="shared" si="6"/>
-        <v>3.8997600000000001</v>
+        <f t="shared" si="8"/>
+        <v>7.58432</v>
       </c>
       <c r="DW12" s="4">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>3.6039500000000002</v>
       </c>
       <c r="DX12" s="4">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>1.0007999999999999</v>
       </c>
       <c r="DY12" s="4">
-        <f t="shared" si="6"/>
-        <v>8.9715000000000007</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="DZ12" s="4">
-        <f t="shared" si="6"/>
-        <v>14.2028</v>
+        <f t="shared" si="8"/>
+        <v>8.7178100000000001</v>
       </c>
       <c r="EA12" s="4">
-        <f t="shared" si="6"/>
-        <v>9.2013800000000003</v>
+        <f t="shared" si="8"/>
+        <v>10</v>
       </c>
       <c r="EB12" s="4">
-        <f t="shared" si="6"/>
-        <v>1.29365</v>
-      </c>
-      <c r="EC12" s="3"/>
+        <f t="shared" si="8"/>
+        <v>5.5027999999999997</v>
+      </c>
+      <c r="EC12" s="4">
+        <f t="shared" si="8"/>
+        <v>3.2463500000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:154" x14ac:dyDescent="0.25">
       <c r="L14">
@@ -6816,7 +6838,7 @@
         <v>0</v>
       </c>
       <c r="BV11">
-        <f t="shared" ref="BV11:EG11" si="1">BV7-BV5</f>
+        <f t="shared" ref="BV11:DE11" si="1">BV7-BV5</f>
         <v>0</v>
       </c>
       <c r="BW11">

</xml_diff>